<commit_message>
Added sensor and cleaned up the board
</commit_message>
<xml_diff>
--- a/Hardware/Skin_Sensor/MK1_BOM.xlsx
+++ b/Hardware/Skin_Sensor/MK1_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="11080" windowWidth="16380" windowHeight="8200"/>
+    <workbookView xWindow="17940" yWindow="8240" windowWidth="16380" windowHeight="8200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -51,9 +51,6 @@
     <t>C9,C13</t>
   </si>
   <si>
-    <t>C10,C14</t>
-  </si>
-  <si>
     <t>0603 Cer Cap 100nF</t>
   </si>
   <si>
@@ -199,6 +196,27 @@
   </si>
   <si>
     <t>LNJ247W82RA</t>
+  </si>
+  <si>
+    <t>C3,C10,C14,C28</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>DPS310 Pressure Sensor</t>
+  </si>
+  <si>
+    <t>DPS310XTSA1</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>0402 Res 100k</t>
+  </si>
+  <si>
+    <t>RC0402JR-07100KL</t>
   </si>
 </sst>
 </file>
@@ -253,8 +271,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -274,15 +294,17 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -650,7 +672,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
@@ -664,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -678,231 +700,259 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3">
-        <v>5034800600</v>
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
+        <v>12</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5034800600</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>